<commit_message>
updated board layout to optimize for DFM
</commit_message>
<xml_diff>
--- a/Hardware/Production/JLCSMT_Sample_BOM1.xlsx
+++ b/Hardware/Production/JLCSMT_Sample_BOM1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Documents/eagle/projects/SmartEncoder/Hardware/Production/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6523209-0DEE-F949-A62A-9FD1879D2392}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A1775D-16E2-C54E-967E-E5AD8C97DB8C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23040" windowHeight="9380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Board" localSheetId="0">Sheet1!$F$1:$O$4</definedName>
+    <definedName name="Board" localSheetId="0">Sheet1!$F$1:$O$3</definedName>
+    <definedName name="Board_1" localSheetId="0">Sheet1!$P$1:$Y$7</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
@@ -24,8 +25,24 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{E372B759-2663-1E40-8276-F2CE2FE82ADF}" name="Board" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/daniel/Documents/eagle/projects/SmartEncoder/Board.csv" decimal="," thousands="." comma="1" semicolon="1">
+  <connection id="1" xr16:uid="{E372B759-2663-1E40-8276-F2CE2FE82ADF}" name="Board" type="6" refreshedVersion="6" deleted="1" background="1" saveData="1">
+    <textPr sourceFile="/Users/daniel/Documents/eagle/projects/SmartEncoder/Board.csv" decimal="," thousands="." comma="1" semicolon="1">
+      <textFields count="10">
+        <textField type="text"/>
+        <textField type="text"/>
+        <textField type="text"/>
+        <textField type="text"/>
+        <textField type="text"/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" xr16:uid="{4EB267FC-7BA7-C94C-9923-B85CE228FBA9}" name="Board1" type="6" refreshedVersion="6" deleted="1" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/daniel/Documents/eagle/projects/SmartEncoder/Hardware/Production/Board.csv" decimal="," thousands="." comma="1" semicolon="1">
       <textFields count="10">
         <textField type="text"/>
         <textField type="text"/>
@@ -44,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Comment</t>
   </si>
@@ -124,6 +141,39 @@
   </si>
   <si>
     <t>0603</t>
+  </si>
+  <si>
+    <t>100n</t>
+  </si>
+  <si>
+    <t>C0402</t>
+  </si>
+  <si>
+    <t>C1, C2</t>
+  </si>
+  <si>
+    <t>C1525</t>
+  </si>
+  <si>
+    <t>4k7</t>
+  </si>
+  <si>
+    <t>R17, R18, R19</t>
+  </si>
+  <si>
+    <t>C25900</t>
+  </si>
+  <si>
+    <t>ATTINY2313A</t>
+  </si>
+  <si>
+    <t>QFN50P400X400X80-21T260N</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>C185530</t>
   </si>
 </sst>
 </file>
@@ -232,6 +282,10 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Board_1" connectionId="2" xr16:uid="{9DE3C29A-3E20-8F4D-8399-B6CC430552E6}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Board" connectionId="1" xr16:uid="{36DA5F08-DFFD-694F-A780-20E5F521DFA9}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -493,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A5:XFD9"/>
+      <selection activeCell="A8" sqref="A8:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -511,9 +565,15 @@
     <col min="11" max="11" width="39.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -531,8 +591,13 @@
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:20">
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
@@ -546,8 +611,12 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:20">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -565,25 +634,87 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:20">
       <c r="A4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D7" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>